<commit_message>
Added area and hobli wise data validation using gemini
</commit_message>
<xml_diff>
--- a/Baanknetbot/Baanknetextract.xlsx
+++ b/Baanknetbot/Baanknetextract.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,11 +543,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>86616-Canara Bank-</t>
+          <t>90376-Canara Bank-</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>86616</v>
+        <v>90376</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -555,11 +555,11 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>8580000</v>
+        <v>641500</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>J P NAGAR 4TH PHASE</t>
+          <t>BEGUR</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -568,7 +568,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>85800000</v>
+        <v>6415000</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -577,7 +577,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>SITE NO 348 9TH MAIN ROAD DOLLARS COLONY J P NAGAR 4TH PHASE BENGALURU 560078</t>
+          <t>All that piece and parcel of the Property residential Site 
+No.202, formed in Converted Sy. No. 113, (converted 
+for residential purposes under official memorandum No. 
+ALN:SR(S)270/80-81, dated 05-09-1980, issued by the 
+special Deputy Commissioner, Bangalore Urban Dist. 
+Bangalore) Presently bearing BBMP Khatha No. 291/202,
+situated at Begur village, BegurHobli, Bangalore, South 
+Taluk, Presently within BBMP Begur, Ward No. 192, 
+measuring East to West 120 feet and North to south 60 
+feet, and bounded on the: 
+ East by :Basapura Village, 
+ West by: Road, 
+ North by : Site No. 203, 
+ South by: Site No. 201.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -592,12 +605,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>J P NAGAR 4TH PHASE</t>
+          <t>BEGUR</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>M PAWAN KUMAR</t>
+          <t>MALLELLA INFRASRUCTURE PVT LTD`</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -607,7 +620,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Villa</t>
+          <t>Plot</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -617,12 +630,12 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>25-02-2025 14:30</t>
+          <t>20-02-2025 14:30</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>25-02-2025 14:30</t>
+          <t>20-02-2025 14:30</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -632,7 +645,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/229215</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/230502</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -644,23 +657,23 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>82454-State Bank of India-</t>
+          <t>90378-Canara Bank-</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>82454</v>
+        <v>90378</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>State Bank of India</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>280000</v>
+        <v>623000</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>KODIPALYA</t>
+          <t>BEGUR</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -669,16 +682,29 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>2800000</v>
+        <v>6230000</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>9886986418</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>FLAT NO 302, 2ND FLOOR, ANNAPOORNESHWARI RESIDENCY , KODIPALYA , KENGERI HOBLI , BANGALORE-560060 .</t>
+          <t>All that piece and parcel of the Property residential Site 
+No.203, formed in Converted Sy. No. 113, (converted 
+for residential purposes under official memorandum No. 
+ALN:SR(S)270/80-81, dated 05-09-1980, issued by the 
+special Deputy Commissioner, Bangalore Urban Dist. 
+Bangalore) Presently bearing BBMP Khatha No. 633/203, 
+situated at Begur village, BegurHobli, Bangalore, South 
+Taluk, Presently within BBMP Begur, Ward No. 192, 
+measuring East to West 120 feet and North to south 60 
+feet, and bounded on the: 
+ East by :Basapura Village, 
+ West by: Road, 
+ North by : Site No. 204, 
+ South by: Site No. 202.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -693,12 +719,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>KODIPALYA</t>
+          <t>BEGUR</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>RAKESH S C</t>
+          <t>MALLELLA INFRASTRUCTURE PVT LTD</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -708,7 +734,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Flat</t>
+          <t>Plot</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -718,12 +744,12 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>12-02-2025 11:00</t>
+          <t>20-02-2025 14:30</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>12-02-2025 11:00</t>
+          <t>20-02-2025 14:30</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -733,7 +759,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/228099</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/230508</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -745,23 +771,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>81704-State Bank of India-</t>
+          <t>90369-Canara Bank-</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>81704</v>
+        <v>90369</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>State Bank of India</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2343600</v>
+        <v>641500</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Hoskote</t>
+          <t>BEGUR</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -770,16 +796,28 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>23436000</v>
+        <v>6415000</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>9886986418</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>All that piece and parcel of residential Unit bearing No. 39, ‘E’ katha No. 150200401601420162, situated in the Schedule ‘A’ property and known as “SAMRUDDHI MYSTIC WIND”,  in all measuring 948.9236  square feet of Divided land area 513.5327 square feet of exclusive right to use garden area 467.014 square feet of proportionate undivided land area (common areas) and consisting of Four Bedroom Residential House/Unit comprising of Ground + Two Upper floors with total 3100 square feet of super built up area of unit (including proportionate constructed club, gym, party hall, common area, security room etc) with all rights, appurtenances whatsoever hereunder or underneath or above the surface and bounded on the East by: Plot No. 38, West by: Plot No. 40, North by: Road and South by: Private Property.</t>
+          <t>All that piece and parcel of the Property residential Site 
+No.201, formed in Converted Sy. No. 113, (converted 
+for residential purposes under official memorandum No. 
+ALN:SR(S)270/80-81, dated 05-09-1980, issued by the 
+special Deputy Commissioner, Bangalore Urban Dist. 
+Bangalore) Presently bearing BBMP Khatha No. 290/201, 
+situated at Begur village, BegurHobli, Bangalore, South 
+Taluk, Presently within BBMP Begur, Ward No. 192, 
+measuring East to West 120 feet and North to south 60 
+feet, and bounded on the: 
+ East by :Basapura Village, 
+ West by: Road, 
+ North by : Site No. 202,</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -794,12 +832,12 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Hoskote</t>
+          <t>BEGUR</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>ANCYMOL V</t>
+          <t>MALLELLA INFRASRUCTURE PVT LTD</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -809,7 +847,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Villa</t>
+          <t>Plot</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -819,12 +857,12 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>24-02-2025 11:00</t>
+          <t>20-02-2025 14:30</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>24-02-2025 11:00</t>
+          <t>20-02-2025 14:30</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -834,7 +872,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/227784</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/230500</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -846,39 +884,452 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>90365-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>90365</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>534600</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>BEGUR</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>5346000</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>All that piece and parcel of the Property residential Site 
+No.160, BBMP Khatha No.1191/160, (erstwhile Begur 
+Village PanchayathKhatha No.1025, House List 
+No.1183), carved on residential converted land bearing 
+Sy.No. 141, comprised in the comprehensive residential 
+layout known as “Vishwapriya Greeneries”, presently 
+under the administrative jurisdiction of Bruhat 
+Bangalore MahanagaraPalike (BBMP), Begur Ward No. 
+192, situated Begur Village, BegurHobli, Bangalore South 
+Taluk, Bangalore District, Bangalore</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>BEGUR</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>MALLELLA INFRASRUCTURE PVT LTD</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Plot</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>20-02-2025 14:30</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>20-02-2025 14:30</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/230496</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>86616-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>86616</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>8580000</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>J P NAGAR 4TH PHASE</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>85800000</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>SITE NO 348 9TH MAIN ROAD DOLLARS COLONY J P NAGAR 4TH PHASE BENGALURU 560078</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>J P NAGAR 4TH PHASE</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>M PAWAN KUMAR</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Villa</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>25-02-2025 14:30</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>25-02-2025 14:30</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/229215</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>82454-State Bank of India-</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>82454</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>State Bank of India</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>280000</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>KODIPALYA</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2800000</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>9886986418</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>FLAT NO 302, 2ND FLOOR, ANNAPOORNESHWARI RESIDENCY , KODIPALYA , KENGERI HOBLI , BANGALORE-560060 .</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>KODIPALYA</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>RAKESH S C</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>12-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>12-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/228099</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>81704-State Bank of India-</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>81704</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>State Bank of India</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2343600</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Hoskote</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>23436000</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>9886986418</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>All that piece and parcel of residential Unit bearing No. 39, ‘E’ katha No. 150200401601420162, situated in the Schedule ‘A’ property and known as “SAMRUDDHI MYSTIC WIND”,  in all measuring 948.9236  square feet of Divided land area 513.5327 square feet of exclusive right to use garden area 467.014 square feet of proportionate undivided land area (common areas) and consisting of Four Bedroom Residential House/Unit comprising of Ground + Two Upper floors with total 3100 square feet of super built up area of unit (including proportionate constructed club, gym, party hall, common area, security room etc) with all rights, appurtenances whatsoever hereunder or underneath or above the surface and bounded on the East by: Plot No. 38, West by: Plot No. 40, North by: Road and South by: Private Property.</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Hoskote</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>ANCYMOL V</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Villa</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>24-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>24-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/227784</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>76072-Bank of Baroda-</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B9" t="n">
         <v>76072</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Bank of Baroda</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D9" t="n">
         <v>725000</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>kengeri</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="G9" t="n">
         <v>7250000</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>999999999</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>All the piece and parcel of Southern portion of property bearing Site No 11, Municipal Katha No. 1411/11, Measuring East to West:50 Feet and North to South :20 Feet, totally measuring 1000 Sq feet, Situated at Kengeri village, Kengeri Hobli, Bengaluru South Taluk, BBMP, Bengaluru and Bounded as under :
 East by: Road,
@@ -887,204 +1338,204 @@
 South by: Property No 12,</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>kengeri</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>Vijayalaxmi M Hiremath</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
         <is>
           <t>Plot</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>20-02-2025 14:00</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>20-02-2025 14:00</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/225464</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>80767-Bank of India-</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B10" t="n">
         <v>80767</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Bank of India</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D10" t="n">
         <v>1250000</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>byatarayanapura ,mysore road</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="G10" t="n">
         <v>12500000</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>08022959407</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Residential Building consisting of Ground Floor having a plinth area of 1585.00 Sq ft</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>byatarayanapura ,mysore road</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Prashanth Kumar K</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
         <is>
           <t>Individual House</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>15-02-2025 11:00</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>15-02-2025 11:00</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/224674</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>82161-Canara Bank-</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B11" t="n">
         <v>82161</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Canara Bank</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D11" t="n">
         <v>3275100</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="G11" t="n">
         <v>32751000</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>9999999999</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Residential Flat bearing no.701, comprising of 3 BHK, in 7th floor of ‘PRISTINE VARA’ being built in property bearing Muncipal no. 123, situated at Infantry road, Muncipal ward no. 78 of Vasanthnagar, Bengaluru and in all approximately measuring 10397 Sq.Ft. out of 12059 Sq.Ft. and bounded by: East: Road, West: Private property, North: Infantry road and South: Private property  out of which 450 sq.ft. of undivided share, right , title, interest and ownership having super built up area of 2500 Sq.Ft. and carpet area measuring 1665 sq.ft. and right to use common areas such as passages, lobbies, lifts, staircases and other areas of common usage and one covered car parking space in basement bounded on:
 East: By Private property
@@ -1093,305 +1544,712 @@
 South: By Flat no. 702</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>NIKITA PATIL</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>18-02-2025 10:30</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>18-02-2025 10:30</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/224706</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>90416-Bank of India-</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>90416</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Bank of India</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>894100</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>NAYANAPPANA HALLI</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>8941000</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>08022959481</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>FLAT NO 110 JJ ELITA 1ST FLOOR AREKERE RANGE NYANAPPANAHALLI DIVISION AND VILLAGE BENGALURU SOUTH</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>NAYANAPPANA HALLI</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>REGILA IYYA PILLAI</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>25-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>25-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/224318</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>70165-State Bank of India-</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>70165</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>State Bank of India</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>400000</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Kodigehally village</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>9886986418</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Flat No 307, Block-B . " JAI PARK SQUARE APARTMENT "</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Kodigehally village</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Adams kevin gautam</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>14-02-2025 10:00</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>14-02-2025 10:00</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/223394</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>70153-State Bank of India-</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B14" t="n">
         <v>70153</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>State Bank of India</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D14" t="n">
         <v>400000</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>Kodigehally</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="G14" t="n">
         <v>4000000</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>9886986418</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Flat no 207, Block-B, 2nd floor, JAI PARK SQUARE APARTMENT , Kodigehally village , K R Puram hobli, Bangalore-560036.</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>Kodigehally</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>Adams kevin gautam</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>14-02-2025 10:00</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>14-02-2025 10:00</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/223648</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="U14" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>70165-State Bank of India-</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>70165</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>State Bank of India</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>400000</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Kodigehally village</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>93698-Bank of Baroda-</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>93698</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Bank of Baroda</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>529650</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>KENGERI</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G9" t="n">
-        <v>4000000</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>9886986418</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Flat No 307, Block-B . " JAI PARK SQUARE APARTMENT "</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="G15" t="n">
+        <v>5296500</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>999999999</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>RESIDENTIAL APPARTMENT KNOWN AS GURU RESIDENCY FLAT NO S-203 2ND FLOOR SITE NO 176 SITUATED AT MYLASANDRA VILLAGE KENGERI HOBLI BANGALORE 560060</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Kodigehally village</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Adams kevin gautam</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>KENGERI</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>M V UMAMAHESHWARI</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>14-02-2025 10:00</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>14-02-2025 10:00</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/223394</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>06-03-2025 14:00</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>06-03-2025 14:00</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/222906</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>90397-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>90397</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>305700</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>BENGALURU</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>3057000</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>GARDEN RESIDENCY, FLAT NO E 102, JIGANI</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>BENGALURU</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>KCHERIS MARKETING</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>28-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>28-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/220726</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>82367-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>82367</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>520000</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>BANGALORE</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>5200000</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Flat No. 2, first floor, Balaji Enclave – 2, No. 120/204, 5th Main road, Ravi Kirloskar Layout, Chikkabidarakallu Village, Dasanapura Hobli, Bangalore – 560072 measuring 1500 Sft.
+Coordinates of the property 
+Latitude- 13.0535297N
+Longitude- 77.4839286E</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>BANGALORE</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>BANGALORE CONSULTANTS - CONTRACTORS</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>20-02-2025 10:30</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>20-02-2025 10:30</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/220163</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>80941-Canara Bank-</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B18" t="n">
         <v>80941</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Canara Bank</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D18" t="n">
         <v>4450500</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="G18" t="n">
         <v>44505000</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>9999999999</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>Residential site carved out of lands in Sy No. 168 of Kodihalli village, Varthur Hobli, Bengaluru South Taluk converted for residential purpose vide b.DIS.ALN.SR/6362 dated 21.03.1974 now within the limits of BBMP and bearing Municiple No. 168, PID No. 74-1-168 situated at old airport road, Kodihalli, Bengaluru under corporation ward No.74- Jeevana Bhimanagar and the site measuring 1935 sq ft. 
 Boundaries of the site: 
@@ -1402,207 +2260,330 @@
 Owner of the property: Mr. P Roshan.</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>COVALENT</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
         <is>
           <t>Plot</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="Q18" t="inlineStr">
         <is>
           <t>11-02-2025 10:30</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="R18" t="inlineStr">
         <is>
           <t>11-02-2025 10:30</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/220183</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="U18" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>82367-Canara Bank-</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>82367</v>
-      </c>
-      <c r="C11" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>90980-Union Bank of India-</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>90980</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Union Bank of India</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>288600</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>2886000</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>"Schedule “A” Property All that piece and parcel of property bearing the Residentially converted Land measuring 2 Acres and 8 Guntas in Sy No.:108/3(previously portion of Sy No.:108/2, Kachanayakanahalli Village, Jigani Hobli, Anekal Taluk, Bangalore District), bearing RDPR No.:150200103200820885, Property No.:522/108/3, situated at Kachanayakanahalli Village, Hennagara Village Panchayath, Anekal Block, Bangalore District (Land converted for Non-Agricultural Residential purposes vide Official Memorandum dated 11.11.1992 vide No.:B/DIS/ALN/SR(A)/103/1988-89 issued by Special Deputy Commissioner, Bangalore) together with 200 Residential Apartment known as “GARDEN RESIDENCY”, Unit/s in A,B,C,D,E &amp; F Blocks together with Car parking slots and bounded on
+East by: Land in Sy No.:108/2,
+West by : Road, Carved out of Kharab Land,
+North by  : Road, Carved out of Kharab Land,
+South by : Tank Bed.
+Schedule “B” Property
+400 Sq. Ft of undivided Share, Rights, Title and Interest in the Schedule “A” property which is the corresponding undivided share in respect of Schedule “C” Apartment unit.
+Schedule “C” Property
+All that piece and parcel of Residential property compromising One Apartment unit i.e Flat bearing no.:BE-407, measuring a super built area of 1089 Sq.Ft in the Third Floor in ‘E’ Block, along with one covered Card Parking space in the Basement/Surface/Stilt Floor and 400 Sq.Ft of Undivided Share, Rights, Title and Interest situated at Apartment building known as “GARDEN RESIDENCY”, Kachanayakanahalli Village, Hennagara Village  Panchayat, Anekal Taluk, Bengaluru District and Bounded as under:
+East by : Residential Apartment privately numbered as E-408 in the Third Floor of “E” Block,
+West by : Area Open to Sky of the Apartment Building,
+North by : Area Open to Sky of the Apartment Building,
+South by : Common Corridor."</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Robin Antony D Cruze</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>28-02-2025 12:00</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>28-02-2025 12:00</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/219714</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>90988-Union Bank of India-</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>90988</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Union Bank of India</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>288600</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>2886000</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>"Schedule A Property
+All that piece and parcel of property residentially converted land measuring 2 Acres 8 Guntas in Sy.No. 108/3( previously portion of Sy.No. 108/2, Kachanayakanahalli Village, Jigani Hobli, Anekal Taluk, Bangalore District), bearing RDPR No. 150200103200820885, property no, 522/108/3, situated at Kachanayakanahalli Village, Hennagara Village Panchayath, Anekal Block, Bangalore District (land converted for non agricultural residential purposes vide official Memorandum dated 11-11-1992 vide no. B/DIS/ALN/SR(A)/103/1988-89, issued by Special Deputy Commissioner, Bangalore District, Bangalore) and  Bounded on the;
+East by : Land in Sy.No. 108/2,
+West by : Road, carved out of kharab land,
+North by : Road, carved out of kharab land,
+South by : Tank Bed
+Schedule B Property
+400 Sq.Ft of undivided share, right, title and interest of Land in the ‘A’ schedule Property
+ Schedule C Property
+All that piece and parcel of property bearing Flat No. BE 205, totally measuring a super built up area of 1089 Sq.ft in the First Floor in ‘E’ Block along with covered Car Parking space in the Basement/Surface/Stilt Floor numbered as BE 205 along with 400 Sq.Ft of undivided interest in land comprising schedule A property is one of such apartment units/flats in the said Apartment Building “ Garden Residency”, situated at Kachanayakanahalli Village, Jigani Hobli, Anekal Taluk, Bengaluru District, Bengaluru and bounded on :
+East by : Lift Area,
+West by : Residential Apartment privately numbered as E-206 in First Floor of E Block,
+North by : Common Corridor
+South by : Area open to sky of apartment building."</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Gangadaraiah T S</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>28-02-2025 12:00</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>28-02-2025 12:00</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/219723</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>81977-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>81977</v>
+      </c>
+      <c r="C21" t="inlineStr">
         <is>
           <t>Canara Bank</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>520000</v>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="D21" t="n">
+        <v>508200</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G11" t="n">
-        <v>5200000</v>
-      </c>
-      <c r="H11" t="inlineStr">
+      <c r="G21" t="n">
+        <v>5082000</v>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>9999999999</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Flat No. 2, first floor, Balaji Enclave – 2, No. 120/204, 5th Main road, Ravi Kirloskar Layout, Chikkabidarakallu Village, Dasanapura Hobli, Bangalore – 560072 measuring 1500 Sft.
-Coordinates of the property 
-Latitude- 13.0535297N
-Longitude- 77.4839286E</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Bengaluru</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>BANGALORE</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>BANGALORE CONSULTANTS - CONTRACTORS</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>Flat</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>Sarfaesi Auction</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>20-02-2025 10:30</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>20-02-2025 10:30</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/220163</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>81977-Canara Bank-</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>81977</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Canara Bank</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>508200</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>BANGALORE</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Ebkray</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>5082000</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>9999999999</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>Flat No. F-403 3rd floor F block, Sy No.108/3, 108/2, Measuring super built up area of 1089 Sqft along with 400 Sqft of undivided interest in land at Garden Residency Apartment, Bommasandra, Jigani Hobli, Anekal Taluk, Bangalore 560099.
 Boundries: 
@@ -1612,103 +2593,416 @@
 West-Residential apartment privately numbered as F-404.</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="M21" t="inlineStr">
         <is>
           <t>P S B DISTRIBUTORS</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="P21" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="Q21" t="inlineStr">
         <is>
           <t>18-02-2025 10:30</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="R21" t="inlineStr">
         <is>
           <t>18-02-2025 10:30</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/219803</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="U21" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>90484-Bank of Baroda-</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>90484</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Bank of Baroda</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>455000</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>BENGALURU</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>4550000</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>999999999</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>A Two bedroom apartment bearing Flat No 301, in C Block,Situated on the Third Floor of the Building known as 
+ “PRUTHVI ROYAL” Constructed on Schedule ‘A’ Property with a  super built up area of 1229.13 Sq. ft along with one covered car parking space which inclusive of proportionate share in common areas, passages, lobbies, staircases and other areas of common use with 316.78 Square Feet of undivided share, right, title and interest and ownership in the land in Schedule ‘A’ Property and bounded by;
+East by: Lobby,
+West by: Open Space, 
+North by: Flat No 302,
+South by: Open Space,</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>BENGALURU</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Srinidhi V</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>27-02-2025 14:00</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>27-02-2025 14:00</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/219173</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>90448-Bank of Baroda-</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>90448</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Bank of Baroda</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>460000</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>BENGALURU</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>4600000</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>999999999</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>A Two bedroom apartment bearing Flat No 203, in C Block, Situated on the Second Floor of the Building known as 
+ “PRUTHVI ROYAL” Constructed on Schedule ‘A’ Property with a  super built up area of 1232.00 Sq. ft along with one covered car parking space which inclusive of proportionate share in common areas, passages, lobbies, staircases and other areas of common use with 317.28 Square Feet of undivided share, right, title and interest and ownership in the land in Schedule ‘A’ Property and bounded by;
+East by: Flat No C-202,
+West by: Flat No C-204, 
+North by: Entrance Corridor,
+South by: Open to Sky,</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>BENGALURU</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>M RAGHAVENDRA</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>27-02-2025 14:00</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>27-02-2025 14:00</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/219172</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>90390-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>90390</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2390000</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>K R PURAM</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>23900000</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>NO 11 HORAMAVU VILLAGE K R PURAM HOBLI BBMP BANGALORE 560043</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>K R PURAM</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>PRAKRUTHI FOUNDATION</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Individual House</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>28-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>28-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/218970</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
         <is>
           <t>80427-Canara Bank-</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B25" t="n">
         <v>80427</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Canara Bank</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D25" t="n">
         <v>1668600</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>bangalore</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="G25" t="n">
         <v>16686000</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>9999999999</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>Residential flat No A-3, 3rd Floor of the apartment known as SRADDHA TULIP having super built up area of 2100 Sft. with one covered car parking space and 414 Sft. of UDS in landed property bearing converted Site no. 3, Mahadevapura CMC Katha no. 448, and converted site bearing nos. 4 &amp; 5, Mahadevapura CMC Katha no. 449, situated at Jayaram Reddy Layout Kundalahalli Village, K R Puram Hobli, Bangalore  East Taluk measuring 5040 Sft. standing in the name of Smt Judy Sweena Kamal
 Value at Sanction: ₹. 151.60
@@ -1717,664 +3011,1573 @@
 Longitude-  77.42460E</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>bangalore</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="M25" t="inlineStr">
         <is>
           <t>KWIKFIX HOSPITALITY PVT LTD</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="P25" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="Q25" t="inlineStr">
         <is>
           <t>14-02-2025 10:30</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr">
+      <c r="R25" t="inlineStr">
         <is>
           <t>14-02-2025 10:30</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/218662</t>
         </is>
       </c>
-      <c r="U13" t="inlineStr">
+      <c r="U25" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>91117-UCO Bank-</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>91117</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>UCO Bank</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1502000</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>JP Nagar</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>15020000</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>08025320436</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Flat No.303 Having SUper BuiltUparea of 1475 sqft(Carpet area 1306 sqft)</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>JP Nagar</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>K K HARIDAS</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>25-02-2025 10:00</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>25-02-2025 10:00</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/217002</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>93216-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>93216</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2538000</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>BASAVESWARANAGARA BANGALORE</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>25380000</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>RESIDENTIAL APARTMENT FLAT</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>BASAVESWARANAGARA BANGALORE</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>SWABHIMAN HOSPITAL</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>12-03-2025 11:30</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>12-03-2025 11:30</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/213914</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>93221-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>93221</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1589100</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>BAHUBALINAGARA</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>15891000</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>residential flat</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>BAHUBALINAGARA</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>SWABHIMAN HOSPITAL</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>12-03-2025 11:30</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>12-03-2025 11:30</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/213922</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>89119-UCO Bank-</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>89119</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>UCO Bank</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1024000</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Old Airport Road</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>10240000</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>08043472770</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Flat bearing No.G1, Corporation No.127/50, New No.127/51 situated at 6th Floor of the “GEM WELLINGTON APARTMENTS”, Airport Road, Murugesh Palya, Kodihalli Village, Bangalore</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Old Airport Road</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Mr.GOPAL KARTHIK BHARTA</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>25-02-2025 13:00</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>25-02-2025 13:00</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/213971</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>82826-Canara Bank-</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B30" t="n">
         <v>82826</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Canara Bank</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="D30" t="n">
         <v>6330000</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>BANASHANKARI III STAGE</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G14" t="n">
+      <c r="G30" t="n">
         <v>63300000</v>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>9999999999</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>RESIDENTIAL 4 FLOOR INDIVIDUAL HOUSES</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K30" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L30" t="inlineStr">
         <is>
           <t>BANASHANKARI III STAGE</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="M30" t="inlineStr">
         <is>
           <t>AISHWARYAGIRI CONSTRUCTIONS PVT LTD</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
         <is>
           <t>Individual House</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="P30" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="Q30" t="inlineStr">
         <is>
           <t>20-02-2025 12:30</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="R30" t="inlineStr">
         <is>
           <t>20-02-2025 12:30</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/212823</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="U30" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>90476-Bank of Baroda-</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>90476</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Bank of Baroda</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>205000</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Adigarakallahalli</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>2050000</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>999999999</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Adigarakallahalli</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Mr.S K MOHAMMED SALIM</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Plot</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>27-02-2025 14:00</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>27-02-2025 14:00</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/207070</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>92908-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>92908</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>401500</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>BANGALORE</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>4015000</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Flat no 404 Third floor SAMPRUTHI ENCLAVE Nagadevanahalli village kengeri hobil situated at padma uadyaya layout , formed in Sy nos 31,32/1 and 35 duly converted into non agricultural land conversion certificate no ALN.SR.2017/1970-71 OF Nagadevanahalli VILLAGE KENGERI HOBIL, Plinth area/Super Built up area for flat 1078 Sq.ft.  Total Carpet area is 808.50 Sq.ft, Undivided area is 254 Sq.ft. PRESENTLY COMING UNDER THE LIMIT OF BBMP AMALGAMATED KHATA NO 2561/2047/4/31,32/1,35/224,223,195 &amp;, 196  and bounded on:
+East: Flat No.403
+West : Road
+North : Flat No.407
+South : Setback</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>BANGALORE</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>MR.HARI RAJ S</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>28-02-2025 10:30</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>28-02-2025 10:30</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/204130</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
         <is>
           <t>82237-Canara Bank-</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B33" t="n">
         <v>82237</v>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>Canara Bank</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D33" t="n">
         <v>287300</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="G33" t="n">
         <v>2873000</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>9999999999</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>Commercial Apartment consisting of unit No 4, 4th floor Sub No.2/15 in the building known as “Narang Chambers” with PID No. 45-47-2/15  Situated at property No.2/3, Ward No 47,  Narasimharaja Road, Bangalore – 560002 measuring super built up area of 415sft with undivided share of 89.52sft and flat bounded on north by Narasimharaja Road South by common passage East by Unit sub numbered 2/16 and west by Unit sub numbered 2/14 and site bounded at North by Narasimharaja road South by conservancy lane East by private property and West by Kumbaragundi property.</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J33" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="K33" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="L33" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="M33" t="inlineStr">
         <is>
           <t>M/S POLYBOND ORGANICS PVT LTD</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="P33" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="Q33" t="inlineStr">
         <is>
           <t>18-02-2025 10:30</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
+      <c r="R33" t="inlineStr">
         <is>
           <t>18-02-2025 10:30</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr">
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/203365</t>
         </is>
       </c>
-      <c r="U15" t="inlineStr">
+      <c r="U33" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="34">
+      <c r="A34" t="inlineStr">
         <is>
           <t>82238-Canara Bank-</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B34" t="n">
         <v>82238</v>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>Canara Bank</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D34" t="n">
         <v>668100</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G16" t="n">
+      <c r="G34" t="n">
         <v>6681000</v>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>9999999999</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>Commercial Apartment consisting of unit No 5, 4th floor Sub No.2/16 in the building known as “Narang Chambers”  Situated at property No.2/3, ward no 47 Narasimharaja Road, Bangalore – 560002 measuring super built up area of 965sft with undivided share of 203.78sft and flat bounded on north by Narasimharaja Road South by Unit sub numbered as 2/17 East by Private property and west by Unit sub numbered 2/15 and site bounded at North by Narasimharaja road South by conservancy lane East by private property and West by Kumbaragundi property.</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="K34" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="L34" t="inlineStr">
         <is>
           <t>BANGALORE</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="M34" t="inlineStr">
         <is>
           <t>M/S POLYBOND ORGANICS PVT LTD</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="P34" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="Q34" t="inlineStr">
         <is>
           <t>18-02-2025 10:30</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="R34" t="inlineStr">
         <is>
           <t>18-02-2025 10:30</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/203375</t>
         </is>
       </c>
-      <c r="U16" t="inlineStr">
+      <c r="U34" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>82842-Canara Bank-</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B35" t="n">
         <v>82842</v>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>Canara Bank</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D35" t="n">
         <v>1290000</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>MILLERS ROAD</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="G35" t="n">
         <v>12900000</v>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>9999999999</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>RESIDENTIAL FLAT</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="J35" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="K35" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="L35" t="inlineStr">
         <is>
           <t>MILLERS ROAD</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="M35" t="inlineStr">
         <is>
           <t>TECHNOSPARK INDUSTRIES INDIA P LTD</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="P35" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
+      <c r="Q35" t="inlineStr">
         <is>
           <t>20-02-2025 11:00</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr">
+      <c r="R35" t="inlineStr">
         <is>
           <t>20-02-2025 11:00</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/203485</t>
         </is>
       </c>
-      <c r="U17" t="inlineStr">
+      <c r="U35" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>90159-Canara Bank-</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>90159</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Canara Bank</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>321600</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>KAMALANAGAR BENGALURU</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>3216000</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>9797408004</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>SITE No- No-575, , Municipal No- 575/41, PID No- 16-54-575/1, carved out of Sy No- 46 of saneguruvanahalli village, situated at BBMP Ward No 16 Kamalanagar, Bengaluru</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>KAMALANAGAR BENGALURU</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>RAJESHWARI R</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Plot</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>01-03-2025 00:00</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>01-03-2025 00:00</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/202782</t>
+        </is>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
         <is>
           <t>84006-Bank of Baroda-</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B37" t="n">
         <v>84006</v>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>Bank of Baroda</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="D37" t="n">
         <v>500000</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>Sarjapur</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="G37" t="n">
         <v>5000000</v>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>999999999</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>Flat No.112,  Pushpam E-town aprtment, Handenahalli</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="J37" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="K37" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="L37" t="inlineStr">
         <is>
           <t>Sarjapur</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="M37" t="inlineStr">
         <is>
           <t>kASILINKA PRADEEP</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
+      <c r="P37" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
+      <c r="Q37" t="inlineStr">
         <is>
           <t>20-02-2025 14:00</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr">
+      <c r="R37" t="inlineStr">
         <is>
           <t>20-02-2025 14:00</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/191155</t>
         </is>
       </c>
-      <c r="U18" t="inlineStr">
+      <c r="U37" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="38">
+      <c r="A38" t="inlineStr">
         <is>
           <t>83988-Bank of Baroda-</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B38" t="n">
         <v>83988</v>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>Bank of Baroda</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D38" t="n">
         <v>570000</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>jAALAHALLI</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>Ebkray</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="G38" t="n">
         <v>5700000</v>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>999999999</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr">
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
         <is>
           <t>Karnataka</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="K38" t="inlineStr">
         <is>
           <t>Bengaluru</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="L38" t="inlineStr">
         <is>
           <t>jAALAHALLI</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="M38" t="inlineStr">
         <is>
           <t>1. PRASHANTHKUMAR 2.kAVITHAKUMARI</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
         <is>
           <t>Flat</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="P38" t="inlineStr">
         <is>
           <t>Sarfaesi Auction</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="Q38" t="inlineStr">
         <is>
           <t>20-02-2025 14:00</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
+      <c r="R38" t="inlineStr">
         <is>
           <t>20-02-2025 14:00</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr">
         <is>
           <t>https://baanknet.com/eauction-psb/api/download-property-document/191150</t>
         </is>
       </c>
-      <c r="U19" t="inlineStr">
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>91684-Union Bank of India-</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>91684</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Union Bank of India</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>279000</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>BENGALURU</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>2790000</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Entire Ground Floor building measuring 830 Sq.Ft of Super Built up area together with 386.66 Sq.Ft of USD situated at BDA No. 824 New Municipal No 824/7 PID No. 23-43-7 6th D Cross Prakashnagar 3rd Stage Rajajinagar BBMP Ward No. 23 Bangalore</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>BENGALURU</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>NAGESH APPYYA  NAYAK</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>28-02-2025 12:00</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>28-02-2025 12:00</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/29723</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>91519-Union Bank of India-</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>91519</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Union Bank of India</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>309900</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>BANGALORE</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Ebkray</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>3099000</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Flat No. S-207 consists of Two bedrooms situated on the 2nd Floor, measuring 1150 Square Feet of Super Built-up area+50 Square Feet of common built-up, along with One Covered Car Parking space in the basement of the Residential Apartment known as VRV ENCLAVE situated Doddabettahalli Village Yelahanka Hobli Bangalore North Taluk Bangalore</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Bengaluru</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>BANGALORE</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>RAVINDRA A</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Flat</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Sarfaesi Auction</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>28-02-2025 12:00</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>28-02-2025 12:00</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/116356</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>

</xml_diff>

<commit_message>
added gemini to find the outstanding amount and possession type of the property
</commit_message>
<xml_diff>
--- a/Baanknetbot/Baanknetextract.xlsx
+++ b/Baanknetbot/Baanknetextract.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U40"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,23 +543,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>90376-Canara Bank-</t>
+          <t>110311-Union Bank of India-</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90376</v>
+        <v>110311</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>Union Bank of India</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>641500</v>
+        <v>386400</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BEGUR</t>
+          <t>Residential</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -568,7 +568,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>6415000</v>
+        <v>3864000</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -577,20 +577,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>All that piece and parcel of the Property residential Site 
-No.202, formed in Converted Sy. No. 113, (converted 
-for residential purposes under official memorandum No. 
-ALN:SR(S)270/80-81, dated 05-09-1980, issued by the 
-special Deputy Commissioner, Bangalore Urban Dist. 
-Bangalore) Presently bearing BBMP Khatha No. 291/202,
-situated at Begur village, BegurHobli, Bangalore, South 
-Taluk, Presently within BBMP Begur, Ward No. 192, 
-measuring East to West 120 feet and North to south 60 
-feet, and bounded on the: 
- East by :Basapura Village, 
- West by: Road, 
- North by : Site No. 203, 
- South by: Site No. 201.</t>
+          <t>Schedule A:All the piece and parcel of the property new Sy. No.223(old Sy. No.173) measuring 2 acres converted vide official memorandum bearing no.ALN(A) SR/107/2010-11 dated 17-03-2010 situated at indlabele village, Attibele Hobli, Anekal Taluk, Bangalore, Schedule B: 507 Sq. Ft of undivided share of right, title and interest and ownership in schedule A, Schedule C: All the piece and parcel of three bedroom residential apartment bearing A-112 of A Block now bearing Bidaraguppe Gramapanchayath E-katha bearing No.150200100200320708, Flat No.248/A-112 on the first floor of the building known as “SIGMA SERENITY” constructed in the Schedule A property, having super built up area of 1375 Sq.Ft(which is inclusive of floors, ceiling and walls between the apartment and portion of share in common areas and a share in common areas and a share in the club house area) together with one covered carparking space in basement.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -605,12 +592,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>BEGUR</t>
+          <t>Residential</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>MALLELLA INFRASRUCTURE PVT LTD`</t>
+          <t>M/s. Chordia Multitrade PVT LTD</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -620,7 +607,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Plot</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -630,12 +617,12 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>20-02-2025 14:30</t>
+          <t>27-03-2025 12:00</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>20-02-2025 14:30</t>
+          <t>27-03-2025 12:00</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -645,7 +632,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/230502</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235872</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -657,23 +644,23 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>90378-Canara Bank-</t>
+          <t>110310-Union Bank of India-</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>90378</v>
+        <v>110310</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>Union Bank of India</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>623000</v>
+        <v>259675</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>BEGUR</t>
+          <t>Residential</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -682,7 +669,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>6230000</v>
+        <v>2596750</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -691,20 +678,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>All that piece and parcel of the Property residential Site 
-No.203, formed in Converted Sy. No. 113, (converted 
-for residential purposes under official memorandum No. 
-ALN:SR(S)270/80-81, dated 05-09-1980, issued by the 
-special Deputy Commissioner, Bangalore Urban Dist. 
-Bangalore) Presently bearing BBMP Khatha No. 633/203, 
-situated at Begur village, BegurHobli, Bangalore, South 
-Taluk, Presently within BBMP Begur, Ward No. 192, 
-measuring East to West 120 feet and North to south 60 
-feet, and bounded on the: 
- East by :Basapura Village, 
- West by: Road, 
- North by : Site No. 204, 
- South by: Site No. 202.</t>
+          <t>Residential apartment bearing No BT-26 in Third floor in Block B of “Ittina Neela” built in schedule property and measuring 1000 sq ft super built up area together with 300 sq ft undivided share, right, title, interest and ownership in the land comprised in schedule A property and a covered car parking in the basement, situated at Andhapura village, Attibele Hobli, Bangalore</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -719,12 +693,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>BEGUR</t>
+          <t>Residential</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>MALLELLA INFRASTRUCTURE PVT LTD</t>
+          <t>Mr. C S Devraj</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -734,7 +708,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Plot</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -744,12 +718,12 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>20-02-2025 14:30</t>
+          <t>27-03-2025 12:00</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>20-02-2025 14:30</t>
+          <t>27-03-2025 12:00</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -759,7 +733,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/230508</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235871</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -771,23 +745,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>90369-Canara Bank-</t>
+          <t>110305-Union Bank of India-</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>90369</v>
+        <v>110305</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>Union Bank of India</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>641500</v>
+        <v>450000</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BEGUR</t>
+          <t>Residential</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -796,7 +770,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>6415000</v>
+        <v>4500000</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -805,19 +779,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>All that piece and parcel of the Property residential Site 
-No.201, formed in Converted Sy. No. 113, (converted 
-for residential purposes under official memorandum No. 
-ALN:SR(S)270/80-81, dated 05-09-1980, issued by the 
-special Deputy Commissioner, Bangalore Urban Dist. 
-Bangalore) Presently bearing BBMP Khatha No. 290/201, 
-situated at Begur village, BegurHobli, Bangalore, South 
-Taluk, Presently within BBMP Begur, Ward No. 192, 
-measuring East to West 120 feet and North to south 60 
-feet, and bounded on the: 
- East by :Basapura Village, 
- West by: Road, 
- North by : Site No. 202,</t>
+          <t>Flat No 103, 1st Floor, Property new BBMP No.8, PID No.95-349-8, Site No. 43 and 43A, Katha No. 1378  and 1379, Krishnappa layout, Shampura New Extension, II block,Shampura village, Kasaba Hobli, Bengaluru 560045</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -832,12 +794,12 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>BEGUR</t>
+          <t>Residential</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>MALLELLA INFRASRUCTURE PVT LTD</t>
+          <t>Mr. Ilyas Ahmad</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -847,7 +809,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Plot</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -857,12 +819,12 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>20-02-2025 14:30</t>
+          <t>27-03-2025 12:00</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>20-02-2025 14:30</t>
+          <t>27-03-2025 12:00</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -872,7 +834,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/230500</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235870</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -884,23 +846,23 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>90365-Canara Bank-</t>
+          <t>110771-State Bank of India-</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>90365</v>
+        <v>110771</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>State Bank of India</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>534600</v>
+        <v>584800</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BEGUR</t>
+          <t>Horamavu,  Bangalore</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -909,25 +871,16 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>5346000</v>
+        <v>5848000</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>9999999999</t>
+          <t>8728072888</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>All that piece and parcel of the Property residential Site 
-No.160, BBMP Khatha No.1191/160, (erstwhile Begur 
-Village PanchayathKhatha No.1025, House List 
-No.1183), carved on residential converted land bearing 
-Sy.No. 141, comprised in the comprehensive residential 
-layout known as “Vishwapriya Greeneries”, presently 
-under the administrative jurisdiction of Bruhat 
-Bangalore MahanagaraPalike (BBMP), Begur Ward No. 
-192, situated Begur Village, BegurHobli, Bangalore South 
-Taluk, Bangalore District, Bangalore</t>
+          <t>Residential APARTMENT/ FLAT No.217 situated in SECOND FLOOR, in the building known and called as “SYCON CRESSIDA” constructed in Schedule ‘L’ Property, having super built up area of 1,075 Square Feet, comprising of TWO bedroom Apartment with ONE Covered Car Parking Space in the Basement of the building with the common right to use the entrance, lobby/s, staircase/s, lift/s, open space, corridors, passages and other areas of common use, together with Water, Electricity and sanitary connections.</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -942,12 +895,12 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>BEGUR</t>
+          <t>Horamavu,  Bangalore</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>MALLELLA INFRASRUCTURE PVT LTD</t>
+          <t>SRINIVASAN  ARUMUGAM</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -957,7 +910,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Plot</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -967,12 +920,12 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>20-02-2025 14:30</t>
+          <t>21-04-2025 11:00</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>20-02-2025 14:30</t>
+          <t>21-04-2025 11:00</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -982,7 +935,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/230496</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235657</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -994,23 +947,23 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>86616-Canara Bank-</t>
+          <t>109660-State Bank of India-</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>86616</v>
+        <v>109660</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>State Bank of India</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8580000</v>
+        <v>720000</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>J P NAGAR 4TH PHASE</t>
+          <t>Anjanapura, Kembathahalli</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1019,16 +972,30 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>85800000</v>
+        <v>7200000</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>9999999999</t>
+          <t>9886986418</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>SITE NO 348 9TH MAIN ROAD DOLLARS COLONY J P NAGAR 4TH PHASE BENGALURU 560078</t>
+          <t>Schedule ‘A’ Property 
+SCHEDULE – I
+All the piece and parcel of land measuring 31 guntas out of 33 guntas, property bearing Sy.No. 61/3, and Sy.No. 60 and Haddigidada land having BDA Khatha No. 61/3, 60 and others situated at Kembathahalli Village, Uttarahalli Hobli, Bengaluru South Taluk, Bengaluru District coming under the limits of BBMP Bengaluru, together with all rights, appurtenance, easements, whatsoever, whether underneath or above the surface, and bounded on:
+East             :   60 Feet Road
+West by       :    BDA site bearing no. 521, 508 and 507 and Road,
+North by   :  Land belonging to Smt. Ratnamma and his son Venugopal and portion of land retained by the owners
+South by      :  30 feet Road.
+                                                                                                         SCHEDULE - II
+(Description of the Undivided Share)
+(Description of the Flat Apartment and undivided share herby conveyed    under this deed)
+431 Sq. feet, of undivided share, right, title and interest in the land comprised in the schedule “A” Property and Residential Apartment no. 2011, on the second floor, of the building known as “SAI NANDNA GP PRIDE”, constructed on the Schedule” A” property, consisting of 2 Bed Rooms and having super built up area of 1175 square feet along with (1) one covered car parking in the basement floor. The walls are built out of solid blocks with vitrified flooring and RCC roofing. It is provided with amenities like electricity, water and sanitary connections and bounded by:
+East by   : Corridor
+West by :  Flat no.2010
+North by : Private property
+South by  : Corridor, staircase and staircase</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1043,12 +1010,12 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>J P NAGAR 4TH PHASE</t>
+          <t>Anjanapura, Kembathahalli</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>M PAWAN KUMAR</t>
+          <t>Sri. Shashidhara Vaichal M</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -1058,7 +1025,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Villa</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -1068,12 +1035,12 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>25-02-2025 14:30</t>
+          <t>19-04-2025 11:00</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>25-02-2025 14:30</t>
+          <t>19-04-2025 11:00</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1083,7 +1050,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/229215</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235665</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1095,23 +1062,23 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>82454-State Bank of India-</t>
+          <t>107228-Central Bank of India-</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>82454</v>
+        <v>107228</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>State Bank of India</t>
+          <t>Central Bank of India</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>280000</v>
+        <v>455000</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>KODIPALYA</t>
+          <t>URBAN</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1120,16 +1087,16 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>2800000</v>
+        <v>4550000</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>9886986418</t>
+          <t>9916102395</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FLAT NO 302, 2ND FLOOR, ANNAPOORNESHWARI RESIDENCY , KODIPALYA , KENGERI HOBLI , BANGALORE-560060 .</t>
+          <t>Flat No.103, First Floor "BHOOMIKA BLUE BELLS" All that part and parcel of property bearing Converted Survey No. 65/1 and 65/2 now assigned new BBMP Katha  No. 932/65/1,65/2 vide conversion certificate bearing No. ALS(SB)(BH)SR26/2012-13 dated 13/02/2014</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1144,12 +1111,12 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>KODIPALYA</t>
+          <t>URBAN</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>RAKESH S C</t>
+          <t>S. MANJUNATH</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1169,12 +1136,12 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>12-02-2025 11:00</t>
+          <t>24-03-2025 10:00</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>12-02-2025 11:00</t>
+          <t>24-03-2025 10:00</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1184,7 +1151,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/228099</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235323</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1196,23 +1163,23 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>81704-State Bank of India-</t>
+          <t>107323-Central Bank of India-</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>81704</v>
+        <v>107323</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>State Bank of India</t>
+          <t>Central Bank of India</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2343600</v>
+        <v>455000</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Hoskote</t>
+          <t>URBAN</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1221,16 +1188,16 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>23436000</v>
+        <v>4550000</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>9886986418</t>
+          <t>9916102395</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>All that piece and parcel of residential Unit bearing No. 39, ‘E’ katha No. 150200401601420162, situated in the Schedule ‘A’ property and known as “SAMRUDDHI MYSTIC WIND”,  in all measuring 948.9236  square feet of Divided land area 513.5327 square feet of exclusive right to use garden area 467.014 square feet of proportionate undivided land area (common areas) and consisting of Four Bedroom Residential House/Unit comprising of Ground + Two Upper floors with total 3100 square feet of super built up area of unit (including proportionate constructed club, gym, party hall, common area, security room etc) with all rights, appurtenances whatsoever hereunder or underneath or above the surface and bounded on the East by: Plot No. 38, West by: Plot No. 40, North by: Road and South by: Private Property.</t>
+          <t>FLAT No. 004, ground floor, BHOOMIKA BLUE BELLS Apartment, S. No. 65/1 and S N. 65/2, BBMP KHATA No. 932/65/1,65/2, Hongasandra Village, Begur Hobli, Bengaluru 560068</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1245,12 +1212,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Hoskote</t>
+          <t>URBAN</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>ANCYMOL V</t>
+          <t>S. MANJUNATHA</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1260,7 +1227,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Villa</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1270,12 +1237,12 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>24-02-2025 11:00</t>
+          <t>24-03-2025 10:00</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>24-02-2025 11:00</t>
+          <t>24-03-2025 10:00</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1285,7 +1252,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/227784</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235341</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1297,23 +1264,23 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>76072-Bank of Baroda-</t>
+          <t>106623-Canara Bank-</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>76072</v>
+        <v>106623</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Bank of Baroda</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>725000</v>
+        <v>1694100</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>kengeri</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1322,20 +1289,19 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>7250000</v>
+        <v>16941000</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>999999999</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>All the piece and parcel of Southern portion of property bearing Site No 11, Municipal Katha No. 1411/11, Measuring East to West:50 Feet and North to South :20 Feet, totally measuring 1000 Sq feet, Situated at Kengeri village, Kengeri Hobli, Bengaluru South Taluk, BBMP, Bengaluru and Bounded as under :
-East by: Road,
-West by: Private property, 
-North by: Northern Portion of Property No 11,
-South by: Property No 12,</t>
+          <t>Property bearing No. F-828, formed in Sy Nos 53/1,53/2,54,56/2,57 to 62/1,62/2, 62/3, 62/4, 62/5, and 62/6, 80/3, 80/-4, 82/1, 82/2, and 82/3, 175,187,189 to 193 vide resolution  No. BDA/TPM/10/397 /88-89 on 25-08-1988 situated at Herohalli Village (Magadi Road) Yeswanthapura Hobli, Bangalore North Taluk, The layout plan approved by BDA and formed by the Bharath Electronics Employees Co-Operative House Building Society Limited, vide Herohalli Panchayath Khatha No. 530,  measuring East by 12.20 Meters West by 12.20 Meters North by 18.30 Meters and south by 18.30 Meters. Bounded by:-  East – Site No. 841/842 West – 40 feet Road North – Site No. 827 South – Site No. 829 and building standing thereon. Total extent of the plot 2400 Sq.ft.
+Coordinates of the property 
+Latitude- 12.58361N
+Longitude- 77.29044E</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1350,12 +1316,12 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>kengeri</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Vijayalaxmi M Hiremath</t>
+          <t>ALPHA GEARS</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1365,7 +1331,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Plot</t>
+          <t>Individual House</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1375,12 +1341,12 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>20-02-2025 14:00</t>
+          <t>09-04-2025 10:30</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>20-02-2025 14:00</t>
+          <t>09-04-2025 10:30</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1390,7 +1356,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/225464</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235139</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1402,23 +1368,23 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>80767-Bank of India-</t>
+          <t>106612-Canara Bank-</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>80767</v>
+        <v>106612</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bank of India</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1250000</v>
+        <v>3076400</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>byatarayanapura ,mysore road</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1427,16 +1393,23 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>12500000</v>
+        <v>30764000</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>08022959407</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Residential Building consisting of Ground Floor having a plinth area of 1585.00 Sq ft</t>
+          <t>All part and parcel of immovable property bearing municipal No 301 (old No. 21/F) situated in Thimmaih Road, Bangalore Mahanagara Palike ward No79, Bangalore Together with all the construction thereon measuring on east 103 feet, on West 99 feet, on North 19 feet and on south 22 feet and 8 inches, Total extent of the land 2232 Sq.ft and Bounded on the:
+East By: premises bearing old No.21/E of Thimmaiah Road
+West By: Premises bearing old No.21 of Thimmaiah Road
+North By: Thimmaiah Road 
+South By: Conservancy.
+Coordinates of the property 
+Latitude- 12.59240N
+Longitude- 77.36109E</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1451,12 +1424,12 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>byatarayanapura ,mysore road</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Prashanth Kumar K</t>
+          <t>JAVEED STEEL</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1476,12 +1449,12 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>15-02-2025 11:00</t>
+          <t>04-04-2025 10:30</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>15-02-2025 11:00</t>
+          <t>04-04-2025 10:30</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1491,7 +1464,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/224674</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235149</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1503,23 +1476,23 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>82161-Canara Bank-</t>
+          <t>107120-Central Bank of India-</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>82161</v>
+        <v>107120</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>Central Bank of India</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3275100</v>
+        <v>718200</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>BANGALORE</t>
+          <t>NAGARBHAVI BANGALORE</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1528,20 +1501,16 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>32751000</v>
+        <v>7182000</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>9999999999</t>
+          <t>9916102337</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Residential Flat bearing no.701, comprising of 3 BHK, in 7th floor of ‘PRISTINE VARA’ being built in property bearing Muncipal no. 123, situated at Infantry road, Muncipal ward no. 78 of Vasanthnagar, Bengaluru and in all approximately measuring 10397 Sq.Ft. out of 12059 Sq.Ft. and bounded by: East: Road, West: Private property, North: Infantry road and South: Private property  out of which 450 sq.ft. of undivided share, right , title, interest and ownership having super built up area of 2500 Sq.Ft. and carpet area measuring 1665 sq.ft. and right to use common areas such as passages, lobbies, lifts, staircases and other areas of common usage and one covered car parking space in basement bounded on:
-East: By Private property
-West: By Private Property
-North: Road 
-South: By Flat no. 702</t>
+          <t>PROPERTY FLAT NO GF 1 GROUND FLOOR SRI SAYUKTHA ENCLAVE SITE NO 146 11TH MAIN ROAD 9TH BLOCK SECOND STAGE NAGARBHAVI BBMP WARD NO 73 BANGALORE 560072</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1556,12 +1525,12 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>BANGALORE</t>
+          <t>NAGARBHAVI BANGALORE</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>NIKITA PATIL</t>
+          <t>PRASHANTH S M</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1581,12 +1550,12 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>18-02-2025 10:30</t>
+          <t>24-03-2025 10:00</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>18-02-2025 10:30</t>
+          <t>24-03-2025 10:00</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1596,7 +1565,7 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/224706</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/235262</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -1608,23 +1577,23 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>90416-Bank of India-</t>
+          <t>104162-Canara Bank-</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>90416</v>
+        <v>104162</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Bank of India</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>894100</v>
+        <v>430000</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>NAYANAPPANA HALLI</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1633,16 +1602,24 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>8941000</v>
+        <v>4300000</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>08022959481</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>FLAT NO 110 JJ ELITA 1ST FLOOR AREKERE RANGE NYANAPPANAHALLI DIVISION AND VILLAGE BENGALURU SOUTH</t>
+          <t>All that piece and parcel of the immovable property bearing New Sy No 14/2, (Old No 14), BBMP Khata No 245/14/2 situated at Doddabettahally Village, AmbaBhavani Temple Road, Veerasandra, YelahankaHobli, Bangalore North Taluk measuring 1 acre 4 guntas or 47916 Sq feet and bounded on the
+East by;Remaining portion of the same survey No 14/2 and private property 
+West by : Road
+North by: Remaining portion of the same survey no 14/2 and 
+South: Private property
+Schedule B:
+325 Sq feet undivided share, right, title, interest and ownership in Schedule A Property
+Schedule C: All that piece and parcel of the 2 Bed Room apartment bearing No 412 in the B Block on the 4th Floor having super built area of 1225 Sq feet along with a covered car parking slot in the apartment building known as “SashankFlorento” constructed in the Schedule A property along with common areas and facility and property in the name of  
+Mr ManjunathKumta.</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1657,12 +1634,12 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>NAYANAPPANA HALLI</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>REGILA IYYA PILLAI</t>
+          <t>MANJUNATH KUMTA</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1682,12 +1659,12 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>25-02-2025 11:00</t>
+          <t>29-03-2025 11:00</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>25-02-2025 11:00</t>
+          <t>29-03-2025 11:00</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -1697,7 +1674,7 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/224318</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/234745</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -1709,23 +1686,23 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>70165-State Bank of India-</t>
+          <t>101967-Canara Bank-</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>70165</v>
+        <v>101967</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>State Bank of India</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>400000</v>
+        <v>780500</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Kodigehally village</t>
+          <t>ATTIBELE HOBLI ANEKAL TALUK</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1734,16 +1711,16 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>4000000</v>
+        <v>7805000</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>9886986418</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Flat No 307, Block-B . " JAI PARK SQUARE APARTMENT "</t>
+          <t>S2 HOMES THE WATER GROVE FLAT NO FF 05 C BLOCK 4TH FLOOR  KAMMASANDRA VILLAGE ATTIBELE HOBLI ANEKAL TALUK BANGALORE</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1758,12 +1735,12 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Kodigehally village</t>
+          <t>ATTIBELE HOBLI ANEKAL TALUK</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Adams kevin gautam</t>
+          <t>ALTAP IBRAHIM SHAIKH</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1783,12 +1760,12 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>14-02-2025 10:00</t>
+          <t>29-03-2025 11:30</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>14-02-2025 10:00</t>
+          <t>29-03-2025 11:30</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1798,7 +1775,7 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/223394</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/234211</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -1810,23 +1787,23 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>70153-State Bank of India-</t>
+          <t>101960-Canara Bank-</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>70153</v>
+        <v>101960</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>State Bank of India</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>400000</v>
+        <v>780500</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Kodigehally</t>
+          <t>ATTIBELE</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1835,16 +1812,16 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>4000000</v>
+        <v>7805000</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>9886986418</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Flat no 207, Block-B, 2nd floor, JAI PARK SQUARE APARTMENT , Kodigehally village , K R Puram hobli, Bangalore-560036.</t>
+          <t>S2 HOMES THE WATER GROVE FLAT NO FF 06 C BLOCK 4TH FLOOR KAMMASANDRA VILLAGE ATTIBELE HOBLI ANEKAL TALUK BANGALORE</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1859,12 +1836,12 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Kodigehally</t>
+          <t>ATTIBELE</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Adams kevin gautam</t>
+          <t>ALTAP IBRAHIM SHAIKH</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1884,12 +1861,12 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>14-02-2025 10:00</t>
+          <t>29-03-2025 11:30</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>14-02-2025 10:00</t>
+          <t>29-03-2025 11:30</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -1899,7 +1876,7 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/223648</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/234207</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
@@ -1911,23 +1888,23 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>93698-Bank of Baroda-</t>
+          <t>111113-Canara Bank-</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>93698</v>
+        <v>111113</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bank of Baroda</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>529650</v>
+        <v>7000</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>KENGERI</t>
+          <t>GOWRIBIDANUR</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1936,16 +1913,16 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>5296500</v>
+        <v>70000</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>999999999</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>RESIDENTIAL APPARTMENT KNOWN AS GURU RESIDENCY FLAT NO S-203 2ND FLOOR SITE NO 176 SITUATED AT MYLASANDRA VILLAGE KENGERI HOBLI BANGALORE 560060</t>
+          <t>Flat No.313, 3rd Floor, Sri Krishna Enclave in land bearing converted Sy. No.111/1, present BBMP Khata No.406, Hoodi Village, K R Puram Hobli, Bangalore East. Total Plinth area is 1523 Sq.ft.</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1960,12 +1937,12 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>KENGERI</t>
+          <t>GOWRIBIDANUR</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>M V UMAMAHESHWARI</t>
+          <t>M/S BHARANI HI TECH AGRO INDUSTRIES</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1985,12 +1962,12 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>06-03-2025 14:00</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>06-03-2025 14:00</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -2000,7 +1977,7 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/222906</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/228480</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
@@ -2012,11 +1989,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>90397-Canara Bank-</t>
+          <t>111153-Canara Bank-</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>90397</v>
+        <v>111153</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -2024,11 +2001,11 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>305700</v>
+        <v>587300</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>BENGALURU</t>
+          <t>K R PURAM</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2037,7 +2014,7 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>3057000</v>
+        <v>5873000</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -2046,7 +2023,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>GARDEN RESIDENCY, FLAT NO E 102, JIGANI</t>
+          <t>Flat No.111, 1st Floor, Sri Krishna sai Enclave in land bearing converted Sy. No.111/1, present BBMP Khata No.406, Hoodi Village, K R Puram Hobli, Bangalore East. Total plinth area is 1250 Sq.ft.</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -2061,12 +2038,12 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>BENGALURU</t>
+          <t>K R PURAM</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>KCHERIS MARKETING</t>
+          <t>M/S BHARANI HI TECH AGRO INDUSTRIES</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -2086,12 +2063,12 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>28-02-2025 11:00</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>28-02-2025 11:00</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -2101,7 +2078,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/220726</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/228494</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -2113,11 +2090,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>82367-Canara Bank-</t>
+          <t>111128-Canara Bank-</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>82367</v>
+        <v>111128</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -2125,11 +2102,11 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>520000</v>
+        <v>583000</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>BANGALORE</t>
+          <t>K R PURAM</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2138,7 +2115,7 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>5200000</v>
+        <v>5830000</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -2147,10 +2124,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Flat No. 2, first floor, Balaji Enclave – 2, No. 120/204, 5th Main road, Ravi Kirloskar Layout, Chikkabidarakallu Village, Dasanapura Hobli, Bangalore – 560072 measuring 1500 Sft.
-Coordinates of the property 
-Latitude- 13.0535297N
-Longitude- 77.4839286E</t>
+          <t>Flat No.203, 2nd Floor, Sri Krishna sai Enclave in land bearing converted Sy. No.111/1, present BBMP Khata No.406, Hoodi Village, K R Puram Hobli, Bangalore East. Total plinth area is 1241 Sq.ft.</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -2165,12 +2139,12 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>BANGALORE</t>
+          <t>K R PURAM</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>BANGALORE CONSULTANTS - CONTRACTORS</t>
+          <t>M/S BHARANI HI TECH AGRO INDUSTRIES</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -2190,12 +2164,12 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>20-02-2025 10:30</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>20-02-2025 10:30</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2205,7 +2179,7 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/220163</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/228483</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
@@ -2217,11 +2191,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>80941-Canara Bank-</t>
+          <t>111139-Canara Bank-</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>80941</v>
+        <v>111139</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -2229,11 +2203,11 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4450500</v>
+        <v>583000</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>BANGALORE</t>
+          <t>K R PURAM</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2242,7 +2216,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>44505000</v>
+        <v>5830000</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -2251,13 +2225,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Residential site carved out of lands in Sy No. 168 of Kodihalli village, Varthur Hobli, Bengaluru South Taluk converted for residential purpose vide b.DIS.ALN.SR/6362 dated 21.03.1974 now within the limits of BBMP and bearing Municiple No. 168, PID No. 74-1-168 situated at old airport road, Kodihalli, Bengaluru under corporation ward No.74- Jeevana Bhimanagar and the site measuring 1935 sq ft. 
-Boundaries of the site: 
-East by: property belonging to Bandiyappa
-West by: Diamond district apartment
-North by: old Airport road 
-South by: Remaining portion of Vinay Kumar 
-Owner of the property: Mr. P Roshan.</t>
+          <t>Flat No.308, 3rd Floor, Sri Krishna sai Enclave in land bearing converted Sy. No.111/1, present BBMP Khata No.406, Hoodi Village, K R Puram Hobli, Bangalore East. Total plinth area is 1241 Sq.ft.</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -2272,12 +2240,12 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>BANGALORE</t>
+          <t>K R PURAM</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>COVALENT</t>
+          <t>M/S BHARANI HI TECH AGRO INDUSTRIES</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -2287,7 +2255,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Plot</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2297,12 +2265,12 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>11-02-2025 10:30</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>11-02-2025 10:30</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -2312,7 +2280,7 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/220183</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/228487</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -2324,19 +2292,19 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>90980-Union Bank of India-</t>
+          <t>112218-UCO Bank-</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>90980</v>
+        <v>112218</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Union Bank of India</t>
+          <t>UCO Bank</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>288600</v>
+        <v>366700</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2349,7 +2317,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>2886000</v>
+        <v>3667000</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -2358,19 +2326,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>"Schedule “A” Property All that piece and parcel of property bearing the Residentially converted Land measuring 2 Acres and 8 Guntas in Sy No.:108/3(previously portion of Sy No.:108/2, Kachanayakanahalli Village, Jigani Hobli, Anekal Taluk, Bangalore District), bearing RDPR No.:150200103200820885, Property No.:522/108/3, situated at Kachanayakanahalli Village, Hennagara Village Panchayath, Anekal Block, Bangalore District (Land converted for Non-Agricultural Residential purposes vide Official Memorandum dated 11.11.1992 vide No.:B/DIS/ALN/SR(A)/103/1988-89 issued by Special Deputy Commissioner, Bangalore) together with 200 Residential Apartment known as “GARDEN RESIDENCY”, Unit/s in A,B,C,D,E &amp; F Blocks together with Car parking slots and bounded on
-East by: Land in Sy No.:108/2,
-West by : Road, Carved out of Kharab Land,
-North by  : Road, Carved out of Kharab Land,
-South by : Tank Bed.
-Schedule “B” Property
-400 Sq. Ft of undivided Share, Rights, Title and Interest in the Schedule “A” property which is the corresponding undivided share in respect of Schedule “C” Apartment unit.
-Schedule “C” Property
-All that piece and parcel of Residential property compromising One Apartment unit i.e Flat bearing no.:BE-407, measuring a super built area of 1089 Sq.Ft in the Third Floor in ‘E’ Block, along with one covered Card Parking space in the Basement/Surface/Stilt Floor and 400 Sq.Ft of Undivided Share, Rights, Title and Interest situated at Apartment building known as “GARDEN RESIDENCY”, Kachanayakanahalli Village, Hennagara Village  Panchayat, Anekal Taluk, Bengaluru District and Bounded as under:
-East by : Residential Apartment privately numbered as E-408 in the Third Floor of “E” Block,
-West by : Area Open to Sky of the Apartment Building,
-North by : Area Open to Sky of the Apartment Building,
-South by : Common Corridor."</t>
+          <t>2 BHK flat having 1030 Sqft</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2390,7 +2346,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Robin Antony D Cruze</t>
+          <t>Balaraj A</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2410,12 +2366,12 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>28-02-2025 12:00</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>28-02-2025 12:00</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -2425,7 +2381,7 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/219714</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/225495</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -2437,23 +2393,23 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>90988-Union Bank of India-</t>
+          <t>110577-Canara Bank-</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>90988</v>
+        <v>110577</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Union Bank of India</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>288600</v>
+        <v>110600</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2462,7 +2418,7 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>2886000</v>
+        <v>1106000</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -2471,20 +2427,13 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>"Schedule A Property
-All that piece and parcel of property residentially converted land measuring 2 Acres 8 Guntas in Sy.No. 108/3( previously portion of Sy.No. 108/2, Kachanayakanahalli Village, Jigani Hobli, Anekal Taluk, Bangalore District), bearing RDPR No. 150200103200820885, property no, 522/108/3, situated at Kachanayakanahalli Village, Hennagara Village Panchayath, Anekal Block, Bangalore District (land converted for non agricultural residential purposes vide official Memorandum dated 11-11-1992 vide no. B/DIS/ALN/SR(A)/103/1988-89, issued by Special Deputy Commissioner, Bangalore District, Bangalore) and  Bounded on the;
-East by : Land in Sy.No. 108/2,
-West by : Road, carved out of kharab land,
-North by : Road, carved out of kharab land,
-South by : Tank Bed
-Schedule B Property
-400 Sq.Ft of undivided share, right, title and interest of Land in the ‘A’ schedule Property
- Schedule C Property
-All that piece and parcel of property bearing Flat No. BE 205, totally measuring a super built up area of 1089 Sq.ft in the First Floor in ‘E’ Block along with covered Car Parking space in the Basement/Surface/Stilt Floor numbered as BE 205 along with 400 Sq.Ft of undivided interest in land comprising schedule A property is one of such apartment units/flats in the said Apartment Building “ Garden Residency”, situated at Kachanayakanahalli Village, Jigani Hobli, Anekal Taluk, Bengaluru District, Bengaluru and bounded on :
-East by : Lift Area,
-West by : Residential Apartment privately numbered as E-206 in First Floor of E Block,
-North by : Common Corridor
-South by : Area open to sky of apartment building."</t>
+          <t>All that piece and parcel of Residential 1 BHK flat in BDA property of Alur Village, Sy No 113 and the total land measuring of 64 houses (including building ) in Block No 35 and 36  measuring East to West 59.20 mtrs, North to South 17.50 mtrs and the property is bounded as follows:
+East by : Road
+West by: BDA Property/Road
+North by: Road
+South by : Passage
+SCHEDULE B PROPERTY:
+Undivided share, right , title interest and ownership in the Schedule A property is 33.526 SqMtrs, total built up area and the total land measuring 1036 Sqmtrs will be shared by all 64 House Owners.</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2499,12 +2448,12 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Gangadaraiah T S</t>
+          <t>MAGESWARA</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -2524,12 +2473,12 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>28-02-2025 12:00</t>
+          <t>29-03-2025 11:00</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>28-02-2025 12:00</t>
+          <t>29-03-2025 11:00</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
@@ -2539,7 +2488,7 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/219723</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/224820</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -2551,11 +2500,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>81977-Canara Bank-</t>
+          <t>110584-Canara Bank-</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>81977</v>
+        <v>110584</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -2563,7 +2512,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>508200</v>
+        <v>241600</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2576,7 +2525,7 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>5082000</v>
+        <v>2416000</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -2585,12 +2534,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Flat No. F-403 3rd floor F block, Sy No.108/3, 108/2, Measuring super built up area of 1089 Sqft along with 400 Sqft of undivided interest in land at Garden Residency Apartment, Bommasandra, Jigani Hobli, Anekal Taluk, Bangalore 560099.
-Boundries: 
-North-common corridor
-South-open to sky of the apartment building
-East-open to sky of the apartment building.
-West-Residential apartment privately numbered as F-404.</t>
+          <t>All that piece and parcel of the property consisting of Flat No 202, Second Floor, “ARYAN RESIDENCY”, measuring 850 sq feet of super built up area, Property bearing Municipal No 28/10, BBMP Ward No 96, PID No 96-71-28/10 ,Old Nos 3 and 4, Gangamma layout, Cholanayakanahally, Guddadahally Main Road, KasabaHobli, Bangalore North Taluk, Bangalore-560032  and property in the name of Mr K V Sridhar andbounded on the 
+As per MODTD                                          As per Valuation report
+East by: Passage                                             East by: Corridor
+West by :Private Property                           West by : Open to sky   
+North by : Flat No 203                                   North by : Flat No 203
+South by:  Flat No 201</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2610,7 +2559,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>P S B DISTRIBUTORS</t>
+          <t>SRIDHAR K V</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2630,12 +2579,12 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>18-02-2025 10:30</t>
+          <t>29-03-2025 11:00</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>18-02-2025 10:30</t>
+          <t>29-03-2025 11:00</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -2645,7 +2594,7 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/219803</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/224830</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
@@ -2657,23 +2606,23 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>90484-Bank of Baroda-</t>
+          <t>97623-Bank of India-</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>90484</v>
+        <v>97623</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bank of Baroda</t>
+          <t>Bank of India</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>455000</v>
+        <v>1125000</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>BENGALURU</t>
+          <t>byatarayanapura ,mysore road</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2682,21 +2631,16 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>4550000</v>
+        <v>11250000</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>999999999</t>
+          <t>08022959407</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>A Two bedroom apartment bearing Flat No 301, in C Block,Situated on the Third Floor of the Building known as 
- “PRUTHVI ROYAL” Constructed on Schedule ‘A’ Property with a  super built up area of 1229.13 Sq. ft along with one covered car parking space which inclusive of proportionate share in common areas, passages, lobbies, staircases and other areas of common use with 316.78 Square Feet of undivided share, right, title and interest and ownership in the land in Schedule ‘A’ Property and bounded by;
-East by: Lobby,
-West by: Open Space, 
-North by: Flat No 302,
-South by: Open Space,</t>
+          <t>Residential Building consisting of Ground Floor having a plinth area of 1585.00 Sq ft</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2711,12 +2655,12 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>BENGALURU</t>
+          <t>byatarayanapura ,mysore road</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Srinidhi V</t>
+          <t>Prashanth Kumar K</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2726,7 +2670,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Flat</t>
+          <t>Individual House</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2736,12 +2680,12 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -2751,7 +2695,7 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/219173</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/224674</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
@@ -2763,23 +2707,23 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>90448-Bank of Baroda-</t>
+          <t>108957-Canara Bank-</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>90448</v>
+        <v>108957</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bank of Baroda</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>460000</v>
+        <v>4005400</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>BENGALURU</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2788,21 +2732,22 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>4600000</v>
+        <v>40054000</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>999999999</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>A Two bedroom apartment bearing Flat No 203, in C Block, Situated on the Second Floor of the Building known as 
- “PRUTHVI ROYAL” Constructed on Schedule ‘A’ Property with a  super built up area of 1232.00 Sq. ft along with one covered car parking space which inclusive of proportionate share in common areas, passages, lobbies, staircases and other areas of common use with 317.28 Square Feet of undivided share, right, title and interest and ownership in the land in Schedule ‘A’ Property and bounded by;
-East by: Flat No C-202,
-West by: Flat No C-204, 
-North by: Entrance Corridor,
-South by: Open to Sky,</t>
+          <t>Residential site carved out of lands in Sy No. 168 of Kodihalli village, Varthur Hobli, Bengaluru South Taluk converted for residential purpose vide b.DIS.ALN.SR/6362 dated 21.03.1974 now within the limits of BBMP and bearing Municiple No. 168, PID No. 74-1-168 situated at old airport road, Kodihalli, Bengaluru under corporation ward No.74- Jeevana Bhimanagar and the site measuring 1935 sq ft. 
+Boundaries of the site: 
+East by: property belonging to Bandiyappa
+West by: Diamond district apartment
+North by: old Airport road 
+South by: Remaining portion of Vinay Kumar 
+Owner of the property: Mr. P Roshan.</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2817,12 +2762,12 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>BENGALURU</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>M RAGHAVENDRA</t>
+          <t>COVALENT</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2832,7 +2777,7 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Flat</t>
+          <t>Plot</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2842,12 +2787,12 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>29-03-2025 10:30</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>29-03-2025 10:30</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
@@ -2857,7 +2802,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/219172</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/220183</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -2869,11 +2814,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>90390-Canara Bank-</t>
+          <t>110993-Canara Bank-</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>90390</v>
+        <v>110993</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -2881,11 +2826,11 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2390000</v>
+        <v>508200</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>K R PURAM</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2894,7 +2839,7 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>23900000</v>
+        <v>5082000</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -2903,7 +2848,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>NO 11 HORAMAVU VILLAGE K R PURAM HOBLI BBMP BANGALORE 560043</t>
+          <t>Flat No. F-403 3rd floor F block, Sy No.108/3, 108/2, Measuring super built up area of 1089 Sqft along with 400 Sqft of undivided interest in land at Garden Residency Apartment, Bommasandra, Jigani Hobli, Anekal Taluk, Bangalore 560099.
+Boundries: 
+North-common corridor
+South-open to sky of the apartment building
+East-open to sky of the apartment building.
+West-Residential apartment privately numbered as F-404.</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2918,12 +2868,12 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>K R PURAM</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>PRAKRUTHI FOUNDATION</t>
+          <t>P S B DISTRIBUTORS</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2933,7 +2883,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Individual House</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2943,12 +2893,12 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>28-02-2025 11:00</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>28-02-2025 11:00</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
@@ -2958,7 +2908,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/218970</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/219803</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -2970,23 +2920,23 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>80427-Canara Bank-</t>
+          <t>97668-Bank of India-</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>80427</v>
+        <v>97668</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>Bank of India</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1668600</v>
+        <v>465500</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>bangalore</t>
+          <t>bommasandra</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2995,20 +2945,16 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>16686000</v>
+        <v>4655000</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>9999999999</t>
+          <t>08022959407</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Residential flat No A-3, 3rd Floor of the apartment known as SRADDHA TULIP having super built up area of 2100 Sft. with one covered car parking space and 414 Sft. of UDS in landed property bearing converted Site no. 3, Mahadevapura CMC Katha no. 448, and converted site bearing nos. 4 &amp; 5, Mahadevapura CMC Katha no. 449, situated at Jayaram Reddy Layout Kundalahalli Village, K R Puram Hobli, Bangalore  East Taluk measuring 5040 Sft. standing in the name of Smt Judy Sweena Kamal
-Value at Sanction: ₹. 151.60
-Coordinates of the property 
-Latitude- 12.57565N
-Longitude-  77.42460E</t>
+          <t>2 BHK Residential flat situated near Bommasandra Industrial area and Electronic city</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -3023,12 +2969,12 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>bangalore</t>
+          <t>bommasandra</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>KWIKFIX HOSPITALITY PVT LTD</t>
+          <t>VISHWANATH MAYYA KC</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -3048,12 +2994,12 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>14-02-2025 10:30</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>14-02-2025 10:30</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -3063,7 +3009,7 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/218662</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/219524</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
@@ -3075,23 +3021,23 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>91117-UCO Bank-</t>
+          <t>97640-Bank of India-</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>91117</v>
+        <v>97640</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>UCO Bank</t>
+          <t>Bank of India</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1502000</v>
+        <v>465500</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>JP Nagar</t>
+          <t>Near Bommasandra Industrial area</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3100,16 +3046,16 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>15020000</v>
+        <v>4655000</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>08025320436</t>
+          <t>08022959407</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Flat No.303 Having SUper BuiltUparea of 1475 sqft(Carpet area 1306 sqft)</t>
+          <t>2 BHK RESIDENTIAL FLAT HAVING A SUPER BUILTUP AREA OF 1089 SQ.FT</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -3124,12 +3070,12 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>JP Nagar</t>
+          <t>Near Bommasandra Industrial area</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>K K HARIDAS</t>
+          <t>Pavithra E</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -3149,12 +3095,12 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>25-02-2025 10:00</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>25-02-2025 10:00</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
@@ -3164,7 +3110,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/217002</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/219588</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -3176,23 +3122,23 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>93216-Canara Bank-</t>
+          <t>98287-Bank of India-</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>93216</v>
+        <v>98287</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>Bank of India</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2538000</v>
+        <v>465500</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>BASAVESWARANAGARA BANGALORE</t>
+          <t>Bommasandra</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3201,16 +3147,16 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>25380000</v>
+        <v>4655000</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>9999999999</t>
+          <t>08022959407</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>RESIDENTIAL APARTMENT FLAT</t>
+          <t>2 BHK residential flat located in 2nd floor,F Block, B tower in the Garden Residency apartment. The Flat is located near Bommasandra Industrial Area</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -3225,12 +3171,12 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>BASAVESWARANAGARA BANGALORE</t>
+          <t>Bommasandra</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>SWABHIMAN HOSPITAL</t>
+          <t>Lekhana B</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -3250,12 +3196,12 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>12-03-2025 11:30</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>12-03-2025 11:30</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -3265,7 +3211,7 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/213914</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/219108</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
@@ -3277,11 +3223,11 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>93221-Canara Bank-</t>
+          <t>109051-Canara Bank-</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>93221</v>
+        <v>109051</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -3289,11 +3235,11 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1589100</v>
+        <v>1668600</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>BAHUBALINAGARA</t>
+          <t>bangalore</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3302,7 +3248,7 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>15891000</v>
+        <v>16686000</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -3311,7 +3257,11 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>residential flat</t>
+          <t>Residential flat No A-3, 3rd Floor of the apartment known as SRADDHA TULIP having super built up area of 2100 Sft. with one covered car parking space and 414 Sft. of UDS in landed property bearing converted Site no. 3, Mahadevapura CMC Katha no. 448, and converted site bearing nos. 4 &amp; 5, Mahadevapura CMC Katha no. 449, situated at Jayaram Reddy Layout Kundalahalli Village, K R Puram Hobli, Bangalore  East Taluk measuring 5040 Sft. standing in the name of Smt Judy Sweena Kamal
+Value at Sanction: ₹. 151.60
+Coordinates of the property 
+Latitude- 12.57565N
+Longitude-  77.42460E</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -3326,12 +3276,12 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>BAHUBALINAGARA</t>
+          <t>bangalore</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>SWABHIMAN HOSPITAL</t>
+          <t>KWIKFIX HOSPITALITY PVT LTD</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -3351,12 +3301,12 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>12-03-2025 11:30</t>
+          <t>29-03-2025 10:30</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>12-03-2025 11:30</t>
+          <t>29-03-2025 10:30</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3366,7 +3316,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/213922</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/218662</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
@@ -3378,23 +3328,23 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>89119-UCO Bank-</t>
+          <t>96186-Central Bank of India-</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>89119</v>
+        <v>96186</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>UCO Bank</t>
+          <t>Central Bank of India</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1024000</v>
+        <v>2800000</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Old Airport Road</t>
+          <t>Bangaluru</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3403,16 +3353,16 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>10240000</v>
+        <v>28000000</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>08043472770</t>
+          <t>8489903009</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Flat bearing No.G1, Corporation No.127/50, New No.127/51 situated at 6th Floor of the “GEM WELLINGTON APARTMENTS”, Airport Road, Murugesh Palya, Kodihalli Village, Bangalore</t>
+          <t>Ground floor AC sheet shed,  Totally measuring  an extent of 3712 Sq. ft. of land at No 50/1, Old No 9/50/1,New BBMP Khatha No 483/474/458/46/9/50/1, Khatha No 50/46/9 South Portion, Sy Nos 46/9 and 46/10, 1st Main, 3rd Cross, KRC Road, Rajiv Gandhi Nagar, Bommanahalli Village, Begur Hobli, Bengaluru 560068.</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -3427,12 +3377,12 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Old Airport Road</t>
+          <t>Bangaluru</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Mr.GOPAL KARTHIK BHARTA</t>
+          <t>M/s Sai Krishna Steel Industries</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -3442,7 +3392,7 @@
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Flat</t>
+          <t>Plot</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -3452,12 +3402,12 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>25-02-2025 13:00</t>
+          <t>24-03-2025 11:00</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>25-02-2025 13:00</t>
+          <t>24-03-2025 11:00</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -3467,7 +3417,7 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/213971</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/213613</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
@@ -3479,11 +3429,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>82826-Canara Bank-</t>
+          <t>110318-Canara Bank-</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>82826</v>
+        <v>110318</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -3553,12 +3503,12 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>20-02-2025 12:30</t>
+          <t>28-03-2025 12:30</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>20-02-2025 12:30</t>
+          <t>28-03-2025 12:30</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -3580,23 +3530,23 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>90476-Bank of Baroda-</t>
+          <t>110903-Canara Bank-</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>90476</v>
+        <v>110903</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bank of Baroda</t>
+          <t>Canara Bank</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>205000</v>
+        <v>287300</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Adigarakallahalli</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3605,14 +3555,18 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>2050000</v>
+        <v>2873000</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>999999999</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr"/>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Commercial Apartment consisting of unit No 4, 4th floor Sub No.2/15 in the building known as “Narang Chambers” with PID No. 45-47-2/15  Situated at property No.2/3, Ward No 47,  Narasimharaja Road, Bangalore – 560002 measuring super built up area of 415sft with undivided share of 89.52sft and flat bounded on north by Narasimharaja Road South by common passage East by Unit sub numbered 2/16 and west by Unit sub numbered 2/14 and site bounded at North by Narasimharaja road South by conservancy lane East by private property and West by Kumbaragundi property.</t>
+        </is>
+      </c>
       <c r="J31" t="inlineStr">
         <is>
           <t>Karnataka</t>
@@ -3625,12 +3579,12 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Adigarakallahalli</t>
+          <t>BANGALORE</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Mr.S K MOHAMMED SALIM</t>
+          <t>M/S POLYBOND ORGANICS PVT LTD</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -3640,7 +3594,7 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Plot</t>
+          <t>Flat</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3650,12 +3604,12 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
@@ -3665,7 +3619,7 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/207070</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/203365</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
@@ -3677,11 +3631,11 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>92908-Canara Bank-</t>
+          <t>110907-Canara Bank-</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>92908</v>
+        <v>110907</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -3689,7 +3643,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>401500</v>
+        <v>668100</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -3702,7 +3656,7 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>4015000</v>
+        <v>6681000</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -3711,11 +3665,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Flat no 404 Third floor SAMPRUTHI ENCLAVE Nagadevanahalli village kengeri hobil situated at padma uadyaya layout , formed in Sy nos 31,32/1 and 35 duly converted into non agricultural land conversion certificate no ALN.SR.2017/1970-71 OF Nagadevanahalli VILLAGE KENGERI HOBIL, Plinth area/Super Built up area for flat 1078 Sq.ft.  Total Carpet area is 808.50 Sq.ft, Undivided area is 254 Sq.ft. PRESENTLY COMING UNDER THE LIMIT OF BBMP AMALGAMATED KHATA NO 2561/2047/4/31,32/1,35/224,223,195 &amp;, 196  and bounded on:
-East: Flat No.403
-West : Road
-North : Flat No.407
-South : Setback</t>
+          <t>Commercial Apartment consisting of unit No 5, 4th floor Sub No.2/16 in the building known as “Narang Chambers”  Situated at property No.2/3, ward no 47 Narasimharaja Road, Bangalore – 560002 measuring super built up area of 965sft with undivided share of 203.78sft and flat bounded on north by Narasimharaja Road South by Unit sub numbered as 2/17 East by Private property and west by Unit sub numbered 2/15 and site bounded at North by Narasimharaja road South by conservancy lane East by private property and West by Kumbaragundi property.</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -3735,7 +3685,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>MR.HARI RAJ S</t>
+          <t>M/S POLYBOND ORGANICS PVT LTD</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -3755,12 +3705,12 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>28-02-2025 10:30</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>28-02-2025 10:30</t>
+          <t>07-04-2025 10:30</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
@@ -3770,7 +3720,7 @@
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/204130</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/203375</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
@@ -3782,11 +3732,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>82237-Canara Bank-</t>
+          <t>110569-Canara Bank-</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>82237</v>
+        <v>110569</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -3794,11 +3744,11 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>287300</v>
+        <v>289400</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>BANGALORE</t>
+          <t>KAMALANAGAR BENGALURU</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3807,16 +3757,20 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>2873000</v>
+        <v>2894000</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>9999999999</t>
+          <t>9797408004</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Commercial Apartment consisting of unit No 4, 4th floor Sub No.2/15 in the building known as “Narang Chambers” with PID No. 45-47-2/15  Situated at property No.2/3, Ward No 47,  Narasimharaja Road, Bangalore – 560002 measuring super built up area of 415sft with undivided share of 89.52sft and flat bounded on north by Narasimharaja Road South by common passage East by Unit sub numbered 2/16 and west by Unit sub numbered 2/14 and site bounded at North by Narasimharaja road South by conservancy lane East by private property and West by Kumbaragundi property.</t>
+          <t>All that part and parcel of the Northern portion of the Site bearing No 575, Municipal No 575/1, PID No 16-54-575/1, carved out of Sy No 46, Saneguruvanahally, BBMP Ward No 16, Kamalanagar, Bangalore measuring East to West 40 feet and North to South 15 feet in all measuring 600 sq feet in the name of Mrs Rajeshwari R and bounded as under:
+East by    : Road
+West by   : Property No 541
+North by  : Property No 576
+South by  : Property No 575 (remaining portion</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -3831,12 +3785,12 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>BANGALORE</t>
+          <t>KAMALANAGAR BENGALURU</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>M/S POLYBOND ORGANICS PVT LTD</t>
+          <t>RAJESHWARI R</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
@@ -3846,7 +3800,7 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Flat</t>
+          <t>Plot</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3856,12 +3810,12 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>18-02-2025 10:30</t>
+          <t>29-03-2025 11:00</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>18-02-2025 10:30</t>
+          <t>29-03-2025 11:00</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
@@ -3871,7 +3825,7 @@
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/203365</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/202782</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
@@ -3883,11 +3837,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>82238-Canara Bank-</t>
+          <t>94752-Canara Bank-</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>82238</v>
+        <v>94752</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -3895,7 +3849,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>668100</v>
+        <v>840000</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -3908,7 +3862,7 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>6681000</v>
+        <v>8400000</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -3917,7 +3871,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Commercial Apartment consisting of unit No 5, 4th floor Sub No.2/16 in the building known as “Narang Chambers”  Situated at property No.2/3, ward no 47 Narasimharaja Road, Bangalore – 560002 measuring super built up area of 965sft with undivided share of 203.78sft and flat bounded on north by Narasimharaja Road South by Unit sub numbered as 2/17 East by Private property and west by Unit sub numbered 2/15 and site bounded at North by Narasimharaja road South by conservancy lane East by private property and West by Kumbaragundi property.</t>
+          <t>RESIDENTIAL FLAT</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -3937,7 +3891,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>M/S POLYBOND ORGANICS PVT LTD</t>
+          <t>GA DOORS AND MORE</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
@@ -3957,12 +3911,12 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>18-02-2025 10:30</t>
+          <t>28-03-2025 11:00</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>18-02-2025 10:30</t>
+          <t>28-03-2025 11:00</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
@@ -3972,7 +3926,7 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/203375</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/202277</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
@@ -3984,11 +3938,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>82842-Canara Bank-</t>
+          <t>94759-Canara Bank-</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>82842</v>
+        <v>94759</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -3996,11 +3950,11 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1290000</v>
+        <v>840000</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>MILLERS ROAD</t>
+          <t>ELECTRONIC CITY</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4009,7 +3963,7 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>12900000</v>
+        <v>8400000</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -4033,12 +3987,12 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>MILLERS ROAD</t>
+          <t>ELECTRONIC CITY</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>TECHNOSPARK INDUSTRIES INDIA P LTD</t>
+          <t>GA DOORS AND MORE</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
@@ -4058,12 +4012,12 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>20-02-2025 11:00</t>
+          <t>28-03-2025 11:00</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>20-02-2025 11:00</t>
+          <t>28-03-2025 11:00</t>
         </is>
       </c>
       <c r="S35" t="inlineStr">
@@ -4073,7 +4027,7 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/203485</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/202378</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
@@ -4085,23 +4039,23 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>90159-Canara Bank-</t>
+          <t>97569-Bank of India-</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>90159</v>
+        <v>97569</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Canara Bank</t>
+          <t>Bank of India</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>321600</v>
+        <v>1090000</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>KAMALANAGAR BENGALURU</t>
+          <t>cottonpet</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4110,16 +4064,16 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>3216000</v>
+        <v>10900000</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>9797408004</t>
+          <t>08022959407</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>SITE No- No-575, , Municipal No- 575/41, PID No- 16-54-575/1, carved out of Sy No- 46 of saneguruvanahalli village, situated at BBMP Ward No 16 Kamalanagar, Bengaluru</t>
+          <t>Residential building built as Duplex Ground + 2 Upper Floors</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -4134,12 +4088,12 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>KAMALANAGAR BENGALURU</t>
+          <t>cottonpet</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>RAJESHWARI R</t>
+          <t>Pinki Kumari C</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -4149,7 +4103,7 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Plot</t>
+          <t>Individual House</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -4159,12 +4113,12 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>01-03-2025 00:00</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>01-03-2025 00:00</t>
+          <t>25-03-2025 11:00</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -4174,7 +4128,7 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/202782</t>
+          <t>https://baanknet.com/eauction-psb/api/download-property-document/197963</t>
         </is>
       </c>
       <c r="U36" t="inlineStr">
@@ -4186,11 +4140,11 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>84006-Bank of Baroda-</t>
+          <t>111780-Bank of Baroda-</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>84006</v>
+        <v>111780</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -4198,7 +4152,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>500000</v>
+        <v>480000</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -4211,7 +4165,7 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>5000000</v>
+        <v>4800000</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -4260,12 +4214,12 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>20-02-2025 14:00</t>
+          <t>29-03-2025 14:00</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>20-02-2025 14:00</t>
+          <t>29-03-2025 14:00</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
@@ -4287,11 +4241,11 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>83988-Bank of Baroda-</t>
+          <t>111786-Bank of Baroda-</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>83988</v>
+        <v>111786</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -4357,12 +4311,12 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>20-02-2025 14:00</t>
+          <t>29-03-2025 14:00</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>20-02-2025 14:00</t>
+          <t>29-03-2025 14:00</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
@@ -4376,208 +4330,6 @@
         </is>
       </c>
       <c r="U38" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>91684-Union Bank of India-</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>91684</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Union Bank of India</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>279000</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>BENGALURU</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Ebkray</t>
-        </is>
-      </c>
-      <c r="G39" t="n">
-        <v>2790000</v>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>9999999999</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>Entire Ground Floor building measuring 830 Sq.Ft of Super Built up area together with 386.66 Sq.Ft of USD situated at BDA No. 824 New Municipal No 824/7 PID No. 23-43-7 6th D Cross Prakashnagar 3rd Stage Rajajinagar BBMP Ward No. 23 Bangalore</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>Bengaluru</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>BENGALURU</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>NAGESH APPYYA  NAYAK</t>
-        </is>
-      </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>Flat</t>
-        </is>
-      </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>Sarfaesi Auction</t>
-        </is>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>28-02-2025 12:00</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>28-02-2025 12:00</t>
-        </is>
-      </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T39" t="inlineStr">
-        <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/29723</t>
-        </is>
-      </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>Physical</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>91519-Union Bank of India-</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>91519</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Union Bank of India</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>309900</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>BANGALORE</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Ebkray</t>
-        </is>
-      </c>
-      <c r="G40" t="n">
-        <v>3099000</v>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>9999999999</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>Flat No. S-207 consists of Two bedrooms situated on the 2nd Floor, measuring 1150 Square Feet of Super Built-up area+50 Square Feet of common built-up, along with One Covered Car Parking space in the basement of the Residential Apartment known as VRV ENCLAVE situated Doddabettahalli Village Yelahanka Hobli Bangalore North Taluk Bangalore</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>Bengaluru</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>BANGALORE</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>RAVINDRA A</t>
-        </is>
-      </c>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>Flat</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>Sarfaesi Auction</t>
-        </is>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>28-02-2025 12:00</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>28-02-2025 12:00</t>
-        </is>
-      </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="T40" t="inlineStr">
-        <is>
-          <t>https://baanknet.com/eauction-psb/api/download-property-document/116356</t>
-        </is>
-      </c>
-      <c r="U40" t="inlineStr">
         <is>
           <t>Physical</t>
         </is>

</xml_diff>